<commit_message>
Minor fix on template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -87,7 +87,7 @@
     <t>Software source:</t>
   </si>
   <si>
-    <t>https://github.com/auino/crypto2excel</t>
+    <t>https://github.com/auino/cryptocurrencies2excel</t>
   </si>
 </sst>
 </file>
@@ -97,7 +97,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,6 +109,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,18 +139,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,7 +432,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,11 +461,14 @@
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Enhanced update time information
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>My Wallets</t>
   </si>
@@ -111,17 +111,21 @@
   <si>
     <t>Last update:</t>
   </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="[$$-409]#,##0.000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,8 +172,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -246,37 +257,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -309,12 +289,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -359,21 +370,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -386,37 +390,52 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -695,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:C14"/>
+      <selection activeCell="B15" sqref="B15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -715,34 +734,34 @@
       <c r="C1" s="15"/>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="27" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27" t="str">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24" t="str">
         <f>IF(A4="","",INDEX(Data!B$2:B$2000,MATCH(A4,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D4" s="31" t="str">
+      <c r="D4" s="34" t="str">
         <f>IF(A4="","",INDEX(Data!D$2:D$2000,MATCH(A4,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E4" s="32" t="str">
+      <c r="E4" s="28" t="str">
         <f>IF(D4="","",D4*B4)</f>
         <v/>
       </c>
@@ -750,31 +769,31 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
-      <c r="C5" s="23" t="str">
+      <c r="C5" s="21" t="str">
         <f>IF(A5="","",INDEX(Data!B$2:B$2000,MATCH(A5,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D5" s="33" t="str">
+      <c r="D5" s="35" t="str">
         <f>IF(A5="","",INDEX(Data!D$2:D$2000,MATCH(A5,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E5" s="34" t="str">
-        <f t="shared" ref="E5:E13" si="0">IF(D5="","",D5*B5)</f>
+      <c r="E5" s="29" t="str">
+        <f t="shared" ref="E5:E12" si="0">IF(D5="","",D5*B5)</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="17"/>
-      <c r="C6" s="23" t="str">
+      <c r="C6" s="21" t="str">
         <f>IF(A6="","",INDEX(Data!B$2:B$2000,MATCH(A6,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D6" s="33" t="str">
+      <c r="D6" s="35" t="str">
         <f>IF(A6="","",INDEX(Data!D$2:D$2000,MATCH(A6,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E6" s="34" t="str">
+      <c r="E6" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -782,15 +801,15 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="17"/>
-      <c r="C7" s="23" t="str">
+      <c r="C7" s="21" t="str">
         <f>IF(A7="","",INDEX(Data!B$2:B$2000,MATCH(A7,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D7" s="33" t="str">
+      <c r="D7" s="35" t="str">
         <f>IF(A7="","",INDEX(Data!D$2:D$2000,MATCH(A7,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E7" s="34" t="str">
+      <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -798,15 +817,15 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
       <c r="B8" s="17"/>
-      <c r="C8" s="23" t="str">
+      <c r="C8" s="21" t="str">
         <f>IF(A8="","",INDEX(Data!B$2:B$2000,MATCH(A8,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D8" s="33" t="str">
+      <c r="D8" s="35" t="str">
         <f>IF(A8="","",INDEX(Data!D$2:D$2000,MATCH(A8,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E8" s="34" t="str">
+      <c r="E8" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -814,15 +833,15 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="17"/>
-      <c r="C9" s="23" t="str">
+      <c r="C9" s="21" t="str">
         <f>IF(A9="","",INDEX(Data!B$2:B$2000,MATCH(A9,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D9" s="33" t="str">
+      <c r="D9" s="35" t="str">
         <f>IF(A9="","",INDEX(Data!D$2:D$2000,MATCH(A9,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E9" s="34" t="str">
+      <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -830,15 +849,15 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="17"/>
-      <c r="C10" s="23" t="str">
+      <c r="C10" s="21" t="str">
         <f>IF(A10="","",INDEX(Data!B$2:B$2000,MATCH(A10,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D10" s="33" t="str">
+      <c r="D10" s="35" t="str">
         <f>IF(A10="","",INDEX(Data!D$2:D$2000,MATCH(A10,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E10" s="34" t="str">
+      <c r="E10" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -846,15 +865,15 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="17"/>
-      <c r="C11" s="23" t="str">
+      <c r="C11" s="21" t="str">
         <f>IF(A11="","",INDEX(Data!B$2:B$2000,MATCH(A11,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D11" s="33" t="str">
+      <c r="D11" s="35" t="str">
         <f>IF(A11="","",INDEX(Data!D$2:D$2000,MATCH(A11,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E11" s="34" t="str">
+      <c r="E11" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -862,47 +881,50 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="17"/>
-      <c r="C12" s="23" t="str">
+      <c r="C12" s="21" t="str">
         <f>IF(A12="","",INDEX(Data!B$2:B$2000,MATCH(A12,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D12" s="33" t="str">
+      <c r="D12" s="35" t="str">
         <f>IF(A12="","",INDEX(Data!D$2:D$2000,MATCH(A12,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E12" s="34" t="str">
+      <c r="E12" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="24" t="str">
-        <f>IF(A13="","",INDEX(Data!B$2:B$2000,MATCH(A13,Data!C$2:C$2000,0)))</f>
-        <v/>
-      </c>
-      <c r="D13" s="35" t="str">
-        <f>IF(A13="","",INDEX(Data!D$2:D$2000,MATCH(A13,Data!C$2:C$2000,0)))</f>
-        <v/>
-      </c>
-      <c r="E13" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="30"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="33"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39">
+        <f>SUM(E4:E13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="42" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -931,7 +953,7 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="25"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Added support to wallets description, plus conversion currencies different from USD
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="6560" windowWidth="28560" windowHeight="16460" activeTab="2"/>
+    <workbookView xWindow="2360" yWindow="6560" windowWidth="28560" windowHeight="16460"/>
   </bookViews>
   <sheets>
     <sheet name="Wallets" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>My Wallets</t>
   </si>
@@ -126,6 +126,9 @@
   <si>
     <t>R / Price (USD)</t>
   </si>
+  <si>
+    <t>Description</t>
+  </si>
 </sst>
 </file>
 
@@ -137,7 +140,7 @@
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
     <numFmt numFmtId="167" formatCode="[$$-409]#,##0.000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,6 +212,14 @@
     <font>
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -352,7 +363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -462,6 +473,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -747,217 +767,233 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="16" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="15"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="E3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="F3" s="27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="23"/>
-      <c r="C4" s="24" t="str">
+      <c r="C4" s="44"/>
+      <c r="D4" s="24" t="str">
         <f>IF(A4="","",INDEX(Data!B$2:B$2000,MATCH(A4,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D4" s="34" t="str">
+      <c r="E4" s="34" t="str">
         <f>IF(A4="","",INDEX(Data!D$2:D$2000,MATCH(A4,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E4" s="28" t="str">
-        <f>IF(D4="","",D4*B4)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="28" t="str">
+        <f t="shared" ref="F4:F12" si="0">IF(E4="","",E4*B4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
-      <c r="C5" s="21" t="str">
+      <c r="C5" s="45"/>
+      <c r="D5" s="21" t="str">
         <f>IF(A5="","",INDEX(Data!B$2:B$2000,MATCH(A5,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D5" s="35" t="str">
+      <c r="E5" s="35" t="str">
         <f>IF(A5="","",INDEX(Data!D$2:D$2000,MATCH(A5,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E5" s="29" t="str">
-        <f t="shared" ref="E5:E12" si="0">IF(D5="","",D5*B5)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="17"/>
-      <c r="C6" s="21" t="str">
+      <c r="C6" s="45"/>
+      <c r="D6" s="21" t="str">
         <f>IF(A6="","",INDEX(Data!B$2:B$2000,MATCH(A6,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D6" s="35" t="str">
+      <c r="E6" s="35" t="str">
         <f>IF(A6="","",INDEX(Data!D$2:D$2000,MATCH(A6,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E6" s="29" t="str">
+      <c r="F6" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="17"/>
-      <c r="C7" s="21" t="str">
+      <c r="C7" s="45"/>
+      <c r="D7" s="21" t="str">
         <f>IF(A7="","",INDEX(Data!B$2:B$2000,MATCH(A7,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D7" s="35" t="str">
+      <c r="E7" s="35" t="str">
         <f>IF(A7="","",INDEX(Data!D$2:D$2000,MATCH(A7,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E7" s="29" t="str">
+      <c r="F7" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
       <c r="B8" s="17"/>
-      <c r="C8" s="21" t="str">
+      <c r="C8" s="45"/>
+      <c r="D8" s="21" t="str">
         <f>IF(A8="","",INDEX(Data!B$2:B$2000,MATCH(A8,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D8" s="35" t="str">
+      <c r="E8" s="35" t="str">
         <f>IF(A8="","",INDEX(Data!D$2:D$2000,MATCH(A8,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E8" s="29" t="str">
+      <c r="F8" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="17"/>
-      <c r="C9" s="21" t="str">
+      <c r="C9" s="45"/>
+      <c r="D9" s="21" t="str">
         <f>IF(A9="","",INDEX(Data!B$2:B$2000,MATCH(A9,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D9" s="35" t="str">
+      <c r="E9" s="35" t="str">
         <f>IF(A9="","",INDEX(Data!D$2:D$2000,MATCH(A9,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E9" s="29" t="str">
+      <c r="F9" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="17"/>
-      <c r="C10" s="21" t="str">
+      <c r="C10" s="45"/>
+      <c r="D10" s="21" t="str">
         <f>IF(A10="","",INDEX(Data!B$2:B$2000,MATCH(A10,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D10" s="35" t="str">
+      <c r="E10" s="35" t="str">
         <f>IF(A10="","",INDEX(Data!D$2:D$2000,MATCH(A10,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E10" s="29" t="str">
+      <c r="F10" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="17"/>
-      <c r="C11" s="21" t="str">
+      <c r="C11" s="45"/>
+      <c r="D11" s="21" t="str">
         <f>IF(A11="","",INDEX(Data!B$2:B$2000,MATCH(A11,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D11" s="35" t="str">
+      <c r="E11" s="35" t="str">
         <f>IF(A11="","",INDEX(Data!D$2:D$2000,MATCH(A11,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E11" s="29" t="str">
+      <c r="F11" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="17"/>
-      <c r="C12" s="21" t="str">
+      <c r="C12" s="45"/>
+      <c r="D12" s="21" t="str">
         <f>IF(A12="","",INDEX(Data!B$2:B$2000,MATCH(A12,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="D12" s="35" t="str">
+      <c r="E12" s="35" t="str">
         <f>IF(A12="","",INDEX(Data!D$2:D$2000,MATCH(A12,Data!C$2:C$2000,0)))</f>
         <v/>
       </c>
-      <c r="E12" s="29" t="str">
+      <c r="F12" s="29" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="30"/>
       <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="33"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
+      <c r="C13" s="46"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="33"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="37">
-        <f>SUM(E4:E13)</f>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="37">
+        <f>SUM(F4:F13)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="40" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="40" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="41"/>
       <c r="C15" s="41"/>
-      <c r="D15" s="39"/>
+      <c r="D15" s="41"/>
       <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1014,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>

</xml_diff>